<commit_message>
Edited picture and overall
</commit_message>
<xml_diff>
--- a/overall (1).xlsx
+++ b/overall (1).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" tabRatio="810" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" tabRatio="810" firstSheet="13" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="admin" sheetId="8" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <sheet name="log_content" sheetId="32" r:id="rId23"/>
     <sheet name="courseware" sheetId="44" r:id="rId24"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="603">
   <si>
     <t>lecturer_id</t>
   </si>
@@ -1298,6 +1298,675 @@
       </rPr>
       <t> employed by MITRE's sponsors, including those for communications, networking, navigation, radar, and electronic warfare.</t>
     </r>
+  </si>
+  <si>
+    <t>MICHAEL</t>
+  </si>
+  <si>
+    <t>ANCHETA</t>
+  </si>
+  <si>
+    <t>LAJERA</t>
+  </si>
+  <si>
+    <t>ANCHETA@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>JOHN HENRY</t>
+  </si>
+  <si>
+    <t>BELLO</t>
+  </si>
+  <si>
+    <t>SABAN</t>
+  </si>
+  <si>
+    <t>BELLO@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>JUSTIN</t>
+  </si>
+  <si>
+    <t>BRUN</t>
+  </si>
+  <si>
+    <t>NEBRIJA</t>
+  </si>
+  <si>
+    <t>BRUN@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>WILLIAM</t>
+  </si>
+  <si>
+    <t>BUENAVENTURA</t>
+  </si>
+  <si>
+    <t>GENESE</t>
+  </si>
+  <si>
+    <t>BUENAVENTURA@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>ROBERT IAN</t>
+  </si>
+  <si>
+    <t>CABRAL</t>
+  </si>
+  <si>
+    <t>DE LEON</t>
+  </si>
+  <si>
+    <t>CABRAL@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>CARL GERARD</t>
+  </si>
+  <si>
+    <t>CADIZ</t>
+  </si>
+  <si>
+    <t>FLORENDO</t>
+  </si>
+  <si>
+    <t>CADIZ@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>ROGER</t>
+  </si>
+  <si>
+    <t>CAJES JR.</t>
+  </si>
+  <si>
+    <t>DATALIO</t>
+  </si>
+  <si>
+    <t>CAJES JR.@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>SHAIRA MAE</t>
+  </si>
+  <si>
+    <t>COSTALES</t>
+  </si>
+  <si>
+    <t>BUNAO</t>
+  </si>
+  <si>
+    <t>COSTALES@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>VEA DENISSE</t>
+  </si>
+  <si>
+    <t>CUEVAS</t>
+  </si>
+  <si>
+    <t>LITAN</t>
+  </si>
+  <si>
+    <t>CUEVAS@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>PAUL DERICK</t>
+  </si>
+  <si>
+    <t>ENRIQUEZ</t>
+  </si>
+  <si>
+    <t>NOCHE</t>
+  </si>
+  <si>
+    <t>ENRIQUEZ@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>DALE PATRICK</t>
+  </si>
+  <si>
+    <t>LANUZO</t>
+  </si>
+  <si>
+    <t>TOLENTINO</t>
+  </si>
+  <si>
+    <t>LANUZO@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>ANGELENE ROCEL</t>
+  </si>
+  <si>
+    <t>LAUNIO</t>
+  </si>
+  <si>
+    <t>BACAYLAN</t>
+  </si>
+  <si>
+    <t>LAUNIO@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>GELLY ANN</t>
+  </si>
+  <si>
+    <t>MATA</t>
+  </si>
+  <si>
+    <t>FRANCISCO</t>
+  </si>
+  <si>
+    <t>MATA@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>PAOLO GIO</t>
+  </si>
+  <si>
+    <t>MENDIOLA</t>
+  </si>
+  <si>
+    <t>MARTINEZ</t>
+  </si>
+  <si>
+    <t>MENDIOLA@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>KESIAH MAE</t>
+  </si>
+  <si>
+    <t>MIGUEL</t>
+  </si>
+  <si>
+    <t>CARDONA</t>
+  </si>
+  <si>
+    <t>MIGUEL@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>ARLYN GAEL</t>
+  </si>
+  <si>
+    <t>MURILLO</t>
+  </si>
+  <si>
+    <t>MABUTAS</t>
+  </si>
+  <si>
+    <t>MURILLO@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>KENNETH ROGER</t>
+  </si>
+  <si>
+    <t>PANTALEON</t>
+  </si>
+  <si>
+    <t>PANALIGAN</t>
+  </si>
+  <si>
+    <t>PANTALEON@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>JOHN VENN</t>
+  </si>
+  <si>
+    <t>PERANDO</t>
+  </si>
+  <si>
+    <t>MANTALA</t>
+  </si>
+  <si>
+    <t>PERANDO@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>RAUL REXOR</t>
+  </si>
+  <si>
+    <t>PIOQUINTO</t>
+  </si>
+  <si>
+    <t>ROSARIO</t>
+  </si>
+  <si>
+    <t>PIOQUINTO@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>JOSE GABRIEL</t>
+  </si>
+  <si>
+    <t>QUEDDENG</t>
+  </si>
+  <si>
+    <t>SUÑGA</t>
+  </si>
+  <si>
+    <t>QUEDDENG@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>MARCO JERIC</t>
+  </si>
+  <si>
+    <t>ROSALES</t>
+  </si>
+  <si>
+    <t>NAVARRO</t>
+  </si>
+  <si>
+    <t>ROSALES@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>JENNY LIZA</t>
+  </si>
+  <si>
+    <t>SUNGA</t>
+  </si>
+  <si>
+    <t>BATALLA</t>
+  </si>
+  <si>
+    <t>SUNGA@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>BRIAN PAUL</t>
+  </si>
+  <si>
+    <t>ANDAYA</t>
+  </si>
+  <si>
+    <t>ANDAYA@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>HARRY MILLE</t>
+  </si>
+  <si>
+    <t>ANG</t>
+  </si>
+  <si>
+    <t>WANG</t>
+  </si>
+  <si>
+    <t>ANG@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>MARTIN DAVE</t>
+  </si>
+  <si>
+    <t>BADINAS</t>
+  </si>
+  <si>
+    <t>TOBIAS</t>
+  </si>
+  <si>
+    <t>BADINAS@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>MARK JOHNNEL</t>
+  </si>
+  <si>
+    <t>BALEN</t>
+  </si>
+  <si>
+    <t>ALORO</t>
+  </si>
+  <si>
+    <t>BALEN@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>HANS PETER KARL</t>
+  </si>
+  <si>
+    <t>BRUNNER</t>
+  </si>
+  <si>
+    <t>FERRERA</t>
+  </si>
+  <si>
+    <t>BRUNNER@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>DARRYLL D`WAYNE</t>
+  </si>
+  <si>
+    <t>BUSTILLOS</t>
+  </si>
+  <si>
+    <t>CUSTAN</t>
+  </si>
+  <si>
+    <t>BUSTILLOS@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>QAEDA VENETT</t>
+  </si>
+  <si>
+    <t>CINCO</t>
+  </si>
+  <si>
+    <t>CRUZ</t>
+  </si>
+  <si>
+    <t>CINCO@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>BENJAMIN</t>
+  </si>
+  <si>
+    <t>CORTINA III</t>
+  </si>
+  <si>
+    <t>FROYALDE</t>
+  </si>
+  <si>
+    <t>CORTINA III@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>GABRIEL</t>
+  </si>
+  <si>
+    <t>DELA FUENTE</t>
+  </si>
+  <si>
+    <t>VARGAS</t>
+  </si>
+  <si>
+    <t>DELA FUENTE@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>DELOS REYES</t>
+  </si>
+  <si>
+    <t>GARCIA</t>
+  </si>
+  <si>
+    <t>DELOS REYES@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>OTHIEL MARK</t>
+  </si>
+  <si>
+    <t>ENRIJO</t>
+  </si>
+  <si>
+    <t>PRIETO</t>
+  </si>
+  <si>
+    <t>ENRIJO@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>PEACHY ANNE</t>
+  </si>
+  <si>
+    <t>FELICIANO</t>
+  </si>
+  <si>
+    <t>TIGLAO</t>
+  </si>
+  <si>
+    <t>FELICIANO@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>JOSE PAOLO</t>
+  </si>
+  <si>
+    <t>GONZALES</t>
+  </si>
+  <si>
+    <t>FRANCISCO@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>DARYL</t>
+  </si>
+  <si>
+    <t>GUZMAN</t>
+  </si>
+  <si>
+    <t>GUZMAN@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>KHALED</t>
+  </si>
+  <si>
+    <t>HASANEIN</t>
+  </si>
+  <si>
+    <t>SORIANO</t>
+  </si>
+  <si>
+    <t>HASANEIN@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>SAMI</t>
+  </si>
+  <si>
+    <t>IBRAHIM</t>
+  </si>
+  <si>
+    <t>YOUSUF</t>
+  </si>
+  <si>
+    <t>IBRAHIM@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>BYEONGJO</t>
+  </si>
+  <si>
+    <t>KIM</t>
+  </si>
+  <si>
+    <t>KIM@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>MARLON</t>
+  </si>
+  <si>
+    <t>MACABENTA</t>
+  </si>
+  <si>
+    <t>TANGHAL</t>
+  </si>
+  <si>
+    <t>MACABENTA@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>BRIAN</t>
+  </si>
+  <si>
+    <t>MAGADIA</t>
+  </si>
+  <si>
+    <t>CAPISTRANO</t>
+  </si>
+  <si>
+    <t>MAGADIA@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>GABRIEL LUIS</t>
+  </si>
+  <si>
+    <t>MARCELO</t>
+  </si>
+  <si>
+    <t>MARCELO@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>MARIE SHEILA</t>
+  </si>
+  <si>
+    <t>MARTIN</t>
+  </si>
+  <si>
+    <t>MALACAD</t>
+  </si>
+  <si>
+    <t>MARTIN@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>ALAIN VINCENT</t>
+  </si>
+  <si>
+    <t>MINDAÑA</t>
+  </si>
+  <si>
+    <t>ELIZAGA</t>
+  </si>
+  <si>
+    <t>MINDAÑA@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>GERSHOM NORMAN</t>
+  </si>
+  <si>
+    <t>MONTES</t>
+  </si>
+  <si>
+    <t>AJEDO</t>
+  </si>
+  <si>
+    <t>MONTES@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>APPLE JOY</t>
+  </si>
+  <si>
+    <t>OBENARIO</t>
+  </si>
+  <si>
+    <t>CASUNDIN</t>
+  </si>
+  <si>
+    <t>OBENARIO@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>JOAN STEPHEN</t>
+  </si>
+  <si>
+    <t>DUQUE</t>
+  </si>
+  <si>
+    <t>PAZ@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>FERDINAND GABRIEL</t>
+  </si>
+  <si>
+    <t>PERALTA</t>
+  </si>
+  <si>
+    <t>ALHAMBRA</t>
+  </si>
+  <si>
+    <t>PERALTA@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>DALE</t>
+  </si>
+  <si>
+    <t>POLICARPIO</t>
+  </si>
+  <si>
+    <t>REGOSO</t>
+  </si>
+  <si>
+    <t>POLICARPIO@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>JAN LESTER</t>
+  </si>
+  <si>
+    <t>QUINTOS</t>
+  </si>
+  <si>
+    <t>TORRES</t>
+  </si>
+  <si>
+    <t>QUINTOS@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>POJUER KENNETH</t>
+  </si>
+  <si>
+    <t>REYES IV</t>
+  </si>
+  <si>
+    <t>CABALLES</t>
+  </si>
+  <si>
+    <t>REYES IV@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>JOHN MICHAEL</t>
+  </si>
+  <si>
+    <t>SANTOS</t>
+  </si>
+  <si>
+    <t>CATURA</t>
+  </si>
+  <si>
+    <t>SANTOS@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>KEN NICOLE</t>
+  </si>
+  <si>
+    <t>SESE</t>
+  </si>
+  <si>
+    <t>AGUIRRE</t>
+  </si>
+  <si>
+    <t>SESE@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>JEMARSON</t>
+  </si>
+  <si>
+    <t>TIU</t>
+  </si>
+  <si>
+    <t>BERNADINO</t>
+  </si>
+  <si>
+    <t>TIU@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>JOSEF ANGELO</t>
+  </si>
+  <si>
+    <t>TU</t>
+  </si>
+  <si>
+    <t>TU@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>DAIAN</t>
+  </si>
+  <si>
+    <t>VILLA</t>
+  </si>
+  <si>
+    <t>VILLA@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>ANSLEY JANSON</t>
+  </si>
+  <si>
+    <t>YANGA</t>
+  </si>
+  <si>
+    <t>DELA CRUZ</t>
+  </si>
+  <si>
+    <t>YANGA@fit.edu.ph</t>
+  </si>
+  <si>
+    <t>JOHN MCLEIGH</t>
+  </si>
+  <si>
+    <t>YOTOKO</t>
+  </si>
+  <si>
+    <t>REYNOSA</t>
+  </si>
+  <si>
+    <t>YOTOKO@fit.edu.ph</t>
   </si>
 </sst>
 </file>
@@ -1378,7 +2047,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1397,6 +2066,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2307,7 +2979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -3005,7 +3677,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="A21" sqref="A21:K78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3667,10 +4339,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3750,6 +4422,9 @@
       <c r="I2" t="s">
         <v>227</v>
       </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
       <c r="K2">
         <v>1</v>
       </c>
@@ -3782,6 +4457,9 @@
       <c r="I3" t="s">
         <v>227</v>
       </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
       <c r="K3">
         <v>1</v>
       </c>
@@ -3814,6 +4492,9 @@
       <c r="I4" t="s">
         <v>227</v>
       </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
       <c r="K4">
         <v>1</v>
       </c>
@@ -3846,6 +4527,9 @@
       <c r="I5" t="s">
         <v>227</v>
       </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
       <c r="K5">
         <v>1</v>
       </c>
@@ -3878,6 +4562,9 @@
       <c r="I6" t="s">
         <v>227</v>
       </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
       <c r="K6">
         <v>2</v>
       </c>
@@ -3910,6 +4597,9 @@
       <c r="I7" t="s">
         <v>227</v>
       </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
       <c r="K7">
         <v>2</v>
       </c>
@@ -3942,6 +4632,9 @@
       <c r="I8" t="s">
         <v>227</v>
       </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
       <c r="K8">
         <v>2</v>
       </c>
@@ -3974,6 +4667,9 @@
       <c r="I9" t="s">
         <v>227</v>
       </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
       <c r="K9">
         <v>2</v>
       </c>
@@ -4006,6 +4702,9 @@
       <c r="I10" t="s">
         <v>227</v>
       </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
       <c r="K10">
         <v>2</v>
       </c>
@@ -4038,6 +4737,9 @@
       <c r="I11" t="s">
         <v>227</v>
       </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
       <c r="K11">
         <v>3</v>
       </c>
@@ -4070,6 +4772,9 @@
       <c r="I12" t="s">
         <v>227</v>
       </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
       <c r="K12">
         <v>3</v>
       </c>
@@ -4102,6 +4807,9 @@
       <c r="I13" t="s">
         <v>227</v>
       </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
       <c r="K13">
         <v>3</v>
       </c>
@@ -4134,6 +4842,9 @@
       <c r="I14" t="s">
         <v>227</v>
       </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
       <c r="K14">
         <v>3</v>
       </c>
@@ -4166,6 +4877,9 @@
       <c r="I15" t="s">
         <v>227</v>
       </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
       <c r="K15">
         <v>3</v>
       </c>
@@ -4198,6 +4912,9 @@
       <c r="I16" t="s">
         <v>227</v>
       </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
       <c r="K16">
         <v>4</v>
       </c>
@@ -4230,6 +4947,9 @@
       <c r="I17" t="s">
         <v>227</v>
       </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
       <c r="K17">
         <v>4</v>
       </c>
@@ -4262,6 +4982,9 @@
       <c r="I18" t="s">
         <v>227</v>
       </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
       <c r="K18">
         <v>4</v>
       </c>
@@ -4294,6 +5017,9 @@
       <c r="I19" t="s">
         <v>227</v>
       </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
       <c r="K19">
         <v>4</v>
       </c>
@@ -4326,8 +5052,2039 @@
       <c r="I20" t="s">
         <v>227</v>
       </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
       <c r="K20">
         <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="14">
+        <v>201411736</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="G21" t="s">
+        <v>383</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" t="s">
+        <v>227</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="14">
+        <v>201311694</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="G22" t="s">
+        <v>387</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" t="s">
+        <v>227</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="14">
+        <v>201311355</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="G23" t="s">
+        <v>391</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I23" t="s">
+        <v>227</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="14">
+        <v>201412123</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="G24" t="s">
+        <v>395</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I24" t="s">
+        <v>227</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="14">
+        <v>201420066</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>398</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="G25" t="s">
+        <v>399</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I25" t="s">
+        <v>227</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="14">
+        <v>201412338</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>400</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="G26" t="s">
+        <v>403</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I26" t="s">
+        <v>227</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="14">
+        <v>201412224</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>405</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>405</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>405</v>
+      </c>
+      <c r="G27" t="s">
+        <v>407</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I27" t="s">
+        <v>227</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="14">
+        <v>201410821</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>408</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>409</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>410</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>409</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>409</v>
+      </c>
+      <c r="G28" t="s">
+        <v>411</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I28" t="s">
+        <v>227</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="14">
+        <v>201410704</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>414</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="G29" t="s">
+        <v>415</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I29" t="s">
+        <v>227</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="14">
+        <v>201412670</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>416</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="G30" t="s">
+        <v>419</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I30" t="s">
+        <v>227</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="14">
+        <v>201210843</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>422</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="G31" t="s">
+        <v>423</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I31" t="s">
+        <v>227</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="14">
+        <v>201410901</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="G32" t="s">
+        <v>427</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" t="s">
+        <v>227</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="14">
+        <v>201230137</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="G33" t="s">
+        <v>431</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I33" t="s">
+        <v>227</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="14">
+        <v>201410941</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>432</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>433</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>433</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>433</v>
+      </c>
+      <c r="G34" t="s">
+        <v>435</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I34" t="s">
+        <v>227</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="14">
+        <v>201411107</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>436</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>437</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>438</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>437</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>437</v>
+      </c>
+      <c r="G35" t="s">
+        <v>439</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I35" t="s">
+        <v>227</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="14">
+        <v>201412671</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>441</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>441</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>441</v>
+      </c>
+      <c r="G36" t="s">
+        <v>443</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I36" t="s">
+        <v>227</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="14">
+        <v>201411266</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>444</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="G37" t="s">
+        <v>447</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I37" t="s">
+        <v>227</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="14">
+        <v>201412315</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>448</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>449</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>450</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>449</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>449</v>
+      </c>
+      <c r="G38" t="s">
+        <v>451</v>
+      </c>
+      <c r="H38" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I38" t="s">
+        <v>227</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="14">
+        <v>201420024</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>452</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>453</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>454</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>453</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>453</v>
+      </c>
+      <c r="G39" t="s">
+        <v>455</v>
+      </c>
+      <c r="H39" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I39" t="s">
+        <v>227</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="14">
+        <v>201310916</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>457</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>458</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>457</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>457</v>
+      </c>
+      <c r="G40" t="s">
+        <v>459</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I40" t="s">
+        <v>227</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="14">
+        <v>201512691</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="G41" t="s">
+        <v>463</v>
+      </c>
+      <c r="H41" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I41" t="s">
+        <v>227</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="14">
+        <v>201410367</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>464</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>466</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="G42" t="s">
+        <v>467</v>
+      </c>
+      <c r="H42" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I42" t="s">
+        <v>227</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="14">
+        <v>201310584</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>469</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>469</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>469</v>
+      </c>
+      <c r="G43" t="s">
+        <v>470</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I43" t="s">
+        <v>227</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="14">
+        <v>201710117</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>472</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>473</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>472</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>472</v>
+      </c>
+      <c r="G44" t="s">
+        <v>474</v>
+      </c>
+      <c r="H44" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I44" t="s">
+        <v>227</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="14">
+        <v>201710447</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>476</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>477</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>476</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>476</v>
+      </c>
+      <c r="G45" t="s">
+        <v>478</v>
+      </c>
+      <c r="H45" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I45" t="s">
+        <v>227</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="14">
+        <v>201710074</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>479</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>480</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>481</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>480</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>480</v>
+      </c>
+      <c r="G46" t="s">
+        <v>482</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I46" t="s">
+        <v>227</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="14">
+        <v>201710424</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>483</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>484</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>485</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>484</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>484</v>
+      </c>
+      <c r="G47" t="s">
+        <v>486</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I47" t="s">
+        <v>227</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="14">
+        <v>201710100</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>487</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>489</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="G48" t="s">
+        <v>490</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I48" t="s">
+        <v>227</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="14">
+        <v>201710453</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>492</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>493</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>492</v>
+      </c>
+      <c r="F49" s="14" t="s">
+        <v>492</v>
+      </c>
+      <c r="G49" t="s">
+        <v>494</v>
+      </c>
+      <c r="H49" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I49" t="s">
+        <v>227</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="14">
+        <v>201710040</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>495</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="G50" t="s">
+        <v>498</v>
+      </c>
+      <c r="H50" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I50" t="s">
+        <v>227</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="14">
+        <v>201710221</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>499</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>500</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>500</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>500</v>
+      </c>
+      <c r="G51" t="s">
+        <v>502</v>
+      </c>
+      <c r="H51" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" t="s">
+        <v>227</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="14">
+        <v>201710258</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>504</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="G52" t="s">
+        <v>505</v>
+      </c>
+      <c r="H52" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I52" t="s">
+        <v>227</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="14">
+        <v>201710152</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>506</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>507</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>508</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>507</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>507</v>
+      </c>
+      <c r="G53" t="s">
+        <v>509</v>
+      </c>
+      <c r="H53" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I53" t="s">
+        <v>227</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="14">
+        <v>201710057</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>510</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>511</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>512</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>511</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>511</v>
+      </c>
+      <c r="G54" t="s">
+        <v>513</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I54" t="s">
+        <v>227</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="14">
+        <v>201710032</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>514</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>515</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="G55" t="s">
+        <v>516</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I55" t="s">
+        <v>227</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="14">
+        <v>201710042</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>517</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>518</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>504</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>518</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>518</v>
+      </c>
+      <c r="G56" t="s">
+        <v>519</v>
+      </c>
+      <c r="H56" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I56" t="s">
+        <v>227</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="14">
+        <v>201710400</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>520</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>521</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>522</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>521</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>521</v>
+      </c>
+      <c r="G57" t="s">
+        <v>523</v>
+      </c>
+      <c r="H57" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I57" t="s">
+        <v>227</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="14">
+        <v>201710458</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>524</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>525</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>526</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>525</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>525</v>
+      </c>
+      <c r="G58" t="s">
+        <v>527</v>
+      </c>
+      <c r="H58" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I58" t="s">
+        <v>227</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="14">
+        <v>201710365</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>528</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="G59" t="s">
+        <v>530</v>
+      </c>
+      <c r="H59" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I59" t="s">
+        <v>227</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="14">
+        <v>201011240</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>531</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>532</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>533</v>
+      </c>
+      <c r="E60" s="14" t="s">
+        <v>532</v>
+      </c>
+      <c r="F60" s="14" t="s">
+        <v>532</v>
+      </c>
+      <c r="G60" t="s">
+        <v>534</v>
+      </c>
+      <c r="H60" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I60" t="s">
+        <v>227</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="14">
+        <v>201710347</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>536</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>536</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>536</v>
+      </c>
+      <c r="G61" t="s">
+        <v>538</v>
+      </c>
+      <c r="H61" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I61" t="s">
+        <v>227</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="14">
+        <v>201710362</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>539</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>540</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>540</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>540</v>
+      </c>
+      <c r="G62" t="s">
+        <v>541</v>
+      </c>
+      <c r="H62" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I62" t="s">
+        <v>227</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="14">
+        <v>201710368</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>542</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>543</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>544</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>543</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>543</v>
+      </c>
+      <c r="G63" t="s">
+        <v>545</v>
+      </c>
+      <c r="H63" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I63" t="s">
+        <v>227</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="14">
+        <v>201710019</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>546</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>547</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>548</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>547</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>547</v>
+      </c>
+      <c r="G64" t="s">
+        <v>549</v>
+      </c>
+      <c r="H64" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I64" t="s">
+        <v>227</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="14">
+        <v>201710338</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>550</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>551</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>552</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>551</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>551</v>
+      </c>
+      <c r="G65" t="s">
+        <v>553</v>
+      </c>
+      <c r="H65" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I65" t="s">
+        <v>227</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="14">
+        <v>201710050</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>554</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>555</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>556</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>555</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>555</v>
+      </c>
+      <c r="G66" t="s">
+        <v>557</v>
+      </c>
+      <c r="H66" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I66" t="s">
+        <v>227</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" s="14">
+        <v>201710384</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>558</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="F67" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="G67" t="s">
+        <v>560</v>
+      </c>
+      <c r="H67" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I67" t="s">
+        <v>227</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="14">
+        <v>201710054</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>562</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>563</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>562</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>562</v>
+      </c>
+      <c r="G68" t="s">
+        <v>564</v>
+      </c>
+      <c r="H68" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I68" t="s">
+        <v>227</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="14">
+        <v>201710405</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>565</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>566</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>567</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>566</v>
+      </c>
+      <c r="F69" s="14" t="s">
+        <v>566</v>
+      </c>
+      <c r="G69" t="s">
+        <v>568</v>
+      </c>
+      <c r="H69" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I69" t="s">
+        <v>227</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="14">
+        <v>201710174</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>569</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>570</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>571</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>570</v>
+      </c>
+      <c r="F70" s="14" t="s">
+        <v>570</v>
+      </c>
+      <c r="G70" t="s">
+        <v>572</v>
+      </c>
+      <c r="H70" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I70" t="s">
+        <v>227</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="14">
+        <v>201710260</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>573</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>574</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>575</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>574</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>574</v>
+      </c>
+      <c r="G71" t="s">
+        <v>576</v>
+      </c>
+      <c r="H71" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I71" t="s">
+        <v>227</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" s="14">
+        <v>201011434</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>577</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>578</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>579</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>578</v>
+      </c>
+      <c r="F72" s="14" t="s">
+        <v>578</v>
+      </c>
+      <c r="G72" t="s">
+        <v>580</v>
+      </c>
+      <c r="H72" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I72" t="s">
+        <v>227</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" s="14">
+        <v>201412795</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>581</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>582</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>583</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>582</v>
+      </c>
+      <c r="F73" s="14" t="s">
+        <v>582</v>
+      </c>
+      <c r="G73" t="s">
+        <v>584</v>
+      </c>
+      <c r="H73" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I73" t="s">
+        <v>227</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" s="14">
+        <v>201710002</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>585</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>586</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>587</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>586</v>
+      </c>
+      <c r="F74" s="14" t="s">
+        <v>586</v>
+      </c>
+      <c r="G74" t="s">
+        <v>588</v>
+      </c>
+      <c r="H74" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I74" t="s">
+        <v>227</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="K74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" s="14">
+        <v>201111222</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>589</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>590</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>590</v>
+      </c>
+      <c r="F75" s="14" t="s">
+        <v>590</v>
+      </c>
+      <c r="G75" t="s">
+        <v>591</v>
+      </c>
+      <c r="H75" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I75" t="s">
+        <v>227</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="14">
+        <v>201710020</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>592</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>548</v>
+      </c>
+      <c r="E76" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="F76" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="G76" t="s">
+        <v>594</v>
+      </c>
+      <c r="H76" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I76" t="s">
+        <v>227</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="K76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" s="14">
+        <v>201710076</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>595</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>596</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>597</v>
+      </c>
+      <c r="E77" s="14" t="s">
+        <v>596</v>
+      </c>
+      <c r="F77" s="14" t="s">
+        <v>596</v>
+      </c>
+      <c r="G77" t="s">
+        <v>598</v>
+      </c>
+      <c r="H77" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I77" t="s">
+        <v>227</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="K77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" s="14">
+        <v>201710341</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>599</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>601</v>
+      </c>
+      <c r="E78" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="F78" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="G78" t="s">
+        <v>602</v>
+      </c>
+      <c r="H78" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I78" t="s">
+        <v>227</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>